<commit_message>
model bazy danych zmigrowany nazwa bazy danych "budget_application_database"
</commit_message>
<xml_diff>
--- a/dane_uzytkownikow.xlsx
+++ b/dane_uzytkownikow.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,18 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>Kowalscy</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>37b2a3d4-c6fe-4405-839e-a8079dbb2f1c</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Winiary</t>
         </is>
       </c>
     </row>
@@ -469,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +567,44 @@
           <t>b072f231-66e8-47a2-b968-0c53c14ef1e5</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>d604217b-bc10-4be0-af8f-a244f97da735</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jakub</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Zając</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>test@test.pl</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test@test.pl</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>9f86d081884c7d659a2feaa0c55ad015a3bf4f1b2b0b822cd15d6c15b0f00a08</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>37b2a3d4-c6fe-4405-839e-a8079dbb2f1c</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>